<commit_message>
Fix issue with metadata for PCA28 to G12V
</commit_message>
<xml_diff>
--- a/metadata/metadata_all_samples.xlsx
+++ b/metadata/metadata_all_samples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kane9530/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1138F360-2DAF-1749-98B9-8888CE922AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC5A5F71-4247-1740-973B-DE429CB986A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="1140" windowWidth="20140" windowHeight="17280" xr2:uid="{D35927FC-E47B-5C40-9B71-90CEFAE16D93}"/>
   </bookViews>
@@ -975,7 +975,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="2" spans="1:30" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>108</v>

</xml_diff>